<commit_message>
Added a message count script
</commit_message>
<xml_diff>
--- a/Presentatie/CBSdata.xlsx
+++ b/Presentatie/CBSdata.xlsx
@@ -11,6 +11,9 @@
     <sheet name="Blad2" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -63,8 +66,36 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -212,11 +243,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="80557056"/>
-        <c:axId val="49895040"/>
+        <c:axId val="186932736"/>
+        <c:axId val="106203968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80557056"/>
+        <c:axId val="186932736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -246,7 +277,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49895040"/>
+        <c:crossAx val="106203968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -254,7 +285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49895040"/>
+        <c:axId val="106203968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -284,7 +315,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80557056"/>
+        <c:crossAx val="186932736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>

<commit_message>
Added some data and updated the software
</commit_message>
<xml_diff>
--- a/Presentatie/CBSdata.xlsx
+++ b/Presentatie/CBSdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="7740"/>
+    <workbookView xWindow="360" yWindow="150" windowWidth="14355" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -243,11 +243,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="186932736"/>
-        <c:axId val="106203968"/>
+        <c:axId val="178520576"/>
+        <c:axId val="1087730752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="186932736"/>
+        <c:axId val="178520576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -277,7 +277,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106203968"/>
+        <c:crossAx val="1087730752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -285,7 +285,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="106203968"/>
+        <c:axId val="1087730752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -315,7 +315,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="186932736"/>
+        <c:crossAx val="178520576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -657,7 +657,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>